<commit_message>
updated settings.py for database
</commit_message>
<xml_diff>
--- a/sample_service_providers.xlsx
+++ b/sample_service_providers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laxma\OneDrive\Desktop\serviceBuddy\ServiceBuddy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08515C24-822C-43B1-8D88-A370FAC94B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0397164-9763-4B4F-9F0D-665984923F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,9 +486,6 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
@@ -512,9 +509,6 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -590,9 +584,6 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
       <c r="B6" t="s">
         <v>20</v>
       </c>

</xml_diff>